<commit_message>
Lectura de archivo de asistentes de Meetup
</commit_message>
<xml_diff>
--- a/Archivo de prueba Meetup.xlsx
+++ b/Archivo de prueba Meetup.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Pybaq\SAR\Archivos  de prueba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Pybaq\SAR\sar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1280,18 +1281,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1569,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -3220,4 +3210,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>